<commit_message>
added add definition increasing count feature in wcy
</commit_message>
<xml_diff>
--- a/Utility/logindata.xlsx
+++ b/Utility/logindata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\smartcliff_project\Smartcliff_RobotFramework_Project\Utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6143A269-7A99-4AE2-8426-A9217B958889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6252CD-4A49-4DE1-8538-05A0DE9354FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F45ECD97-346C-4BA2-B362-A2663D16A9D0}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371F0178-9731-4D0D-9B6A-D5FB4A29B4BD}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,6 +446,9 @@
         <v>1234</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{9F5679C0-5BA9-4FCD-A8A9-A0D950252082}"/>

</xml_diff>